<commit_message>
Done a lab session, got DataPath B done and started testing
</commit_message>
<xml_diff>
--- a/Homework_1/Instructions.xlsx
+++ b/Homework_1/Instructions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction set" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="123">
   <si>
     <t>Instruction</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>brc</t>
-  </si>
-  <si>
-    <t>Oprands</t>
   </si>
   <si>
     <t>rt,ra,rb</t>
@@ -709,16 +706,10 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -729,9 +720,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -760,21 +748,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -830,6 +817,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
@@ -876,8 +873,8 @@
     <sortCondition descending="1" ref="B2:B11"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Operands" dataDxfId="2"/>
-    <tableColumn id="2" name="Fields" dataDxfId="1"/>
+    <tableColumn id="1" name="Operands" dataDxfId="1"/>
+    <tableColumn id="2" name="Fields" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1151,8 +1148,8 @@
   </sheetPr>
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,16 +1171,16 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="41" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="42" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1192,523 +1189,523 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>108</v>
+      <c r="D3" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="39" t="str">
+        <v>95</v>
+      </c>
+      <c r="G3" s="36" t="str">
         <f>VLOOKUP(D3,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  ΦΦΦΦ ΦΦΦΦ ΦΦΦΦ ΦΦΦΦ</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>47</v>
+      <c r="D4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="38" t="str">
+        <v>70</v>
+      </c>
+      <c r="G4" s="35" t="str">
         <f>VLOOKUP(D4,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  BBBB BAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>48</v>
+      <c r="D5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="40" t="str">
+        <v>71</v>
+      </c>
+      <c r="G5" s="37" t="str">
         <f>VLOOKUP(D5,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  BBBB BAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="44"/>
+      <c r="C6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>49</v>
+      <c r="D6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>48</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="41" t="str">
+        <v>72</v>
+      </c>
+      <c r="G6" s="38" t="str">
         <f>VLOOKUP(D6,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>II IIII IIII  IIII ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>50</v>
+      <c r="D7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="40" t="str">
+        <v>73</v>
+      </c>
+      <c r="G7" s="37" t="str">
         <f>VLOOKUP(D7,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>II IIII IIII  IIII ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="21" t="s">
+      <c r="B8" s="44"/>
+      <c r="C8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>51</v>
+      <c r="D8" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="41" t="str">
+        <v>74</v>
+      </c>
+      <c r="G8" s="38" t="str">
         <f>VLOOKUP(D8,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="24"/>
-      <c r="C9" s="25" t="s">
+      <c r="B9" s="45"/>
+      <c r="C9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>52</v>
+      <c r="D9" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="39" t="str">
+        <v>75</v>
+      </c>
+      <c r="G9" s="36" t="str">
         <f>VLOOKUP(D9,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>53</v>
+      <c r="D10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="38" t="str">
+        <v>86</v>
+      </c>
+      <c r="G10" s="35" t="str">
         <f>VLOOKUP(D10,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>54</v>
+      <c r="D11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="40" t="str">
+        <v>76</v>
+      </c>
+      <c r="G11" s="37" t="str">
         <f>VLOOKUP(D11,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  BBBB BAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>55</v>
+      <c r="D12" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G12" s="41" t="str">
+        <v>77</v>
+      </c>
+      <c r="G12" s="38" t="str">
         <f>VLOOKUP(D12,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  BBBB BAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>56</v>
+      <c r="D13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="40" t="str">
+        <v>78</v>
+      </c>
+      <c r="G13" s="37" t="str">
         <f>VLOOKUP(D13,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  BBBB BAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="17"/>
-      <c r="C14" s="21" t="s">
+      <c r="B14" s="44"/>
+      <c r="C14" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>57</v>
+      <c r="D14" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>56</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="41" t="str">
+        <v>79</v>
+      </c>
+      <c r="G14" s="38" t="str">
         <f>VLOOKUP(D14,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>II IIII IIII  IIII ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>58</v>
+      <c r="D15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="40" t="str">
+        <v>80</v>
+      </c>
+      <c r="G15" s="37" t="str">
         <f>VLOOKUP(D15,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>II IIII IIII  IIII ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="21" t="s">
+      <c r="B16" s="44"/>
+      <c r="C16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>59</v>
+      <c r="D16" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G16" s="41" t="str">
+        <v>81</v>
+      </c>
+      <c r="G16" s="38" t="str">
         <f>VLOOKUP(D16,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>II IIII IIII  IIII ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="18" t="s">
+      <c r="B17" s="44"/>
+      <c r="C17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>60</v>
+      <c r="D17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="40" t="str">
+        <v>84</v>
+      </c>
+      <c r="G17" s="37" t="str">
         <f>VLOOKUP(D17,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ NNNN ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="21" t="s">
+      <c r="B18" s="44"/>
+      <c r="C18" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>61</v>
+      <c r="D18" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>60</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="41" t="str">
+        <v>82</v>
+      </c>
+      <c r="G18" s="38" t="str">
         <f>VLOOKUP(D18,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ NNNN ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="44"/>
+      <c r="C19" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>62</v>
+      <c r="D19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>61</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="40" t="str">
+        <v>83</v>
+      </c>
+      <c r="G19" s="37" t="str">
         <f>VLOOKUP(D19,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ NNNN ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-      <c r="C20" s="28" t="s">
+      <c r="B20" s="45"/>
+      <c r="C20" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>63</v>
+      <c r="D20" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>62</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="42" t="str">
+        <v>85</v>
+      </c>
+      <c r="G20" s="39" t="str">
         <f>VLOOKUP(D20,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ NNNN ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="31" t="s">
+      <c r="B21" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>64</v>
+      <c r="D21" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>63</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="43" t="str">
+        <v>88</v>
+      </c>
+      <c r="G21" s="40" t="str">
         <f>VLOOKUP(D21,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
-      <c r="C22" s="21" t="s">
+      <c r="B22" s="44"/>
+      <c r="C22" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="23" t="s">
-        <v>110</v>
-      </c>
       <c r="F22" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="41" t="str">
+        <v>89</v>
+      </c>
+      <c r="G22" s="38" t="str">
         <f>VLOOKUP(D22,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>AA AAAA AAAA  AAAA AAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="44"/>
+      <c r="C23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>65</v>
+      <c r="D23" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>64</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="G23" s="40" t="str">
+        <v>90</v>
+      </c>
+      <c r="G23" s="37" t="str">
         <f>VLOOKUP(D23,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
-      <c r="C24" s="21" t="s">
+      <c r="B24" s="44"/>
+      <c r="C24" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>66</v>
+      <c r="D24" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="41" t="str">
+        <v>91</v>
+      </c>
+      <c r="G24" s="38" t="str">
         <f>VLOOKUP(D24,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>OO OOOO OOOO  OOOO ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
-      <c r="C25" s="18" t="s">
+      <c r="B25" s="44"/>
+      <c r="C25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>111</v>
+      <c r="D25" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G25" s="40" t="str">
+        <v>92</v>
+      </c>
+      <c r="G25" s="37" t="str">
         <f>VLOOKUP(D25,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>AA AAAA AAAA  AAAA AAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="17"/>
-      <c r="C26" s="21" t="s">
+      <c r="B26" s="44"/>
+      <c r="C26" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>67</v>
+      <c r="D26" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="41" t="str">
+        <v>93</v>
+      </c>
+      <c r="G26" s="38" t="str">
         <f>VLOOKUP(D26,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>ΦΦ ΦΦΦΦ ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="24"/>
-      <c r="C27" s="25" t="s">
+      <c r="B27" s="45"/>
+      <c r="C27" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>68</v>
+      <c r="D27" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G27" s="39" t="str">
+        <v>94</v>
+      </c>
+      <c r="G27" s="36" t="str">
         <f>VLOOKUP(D27,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>OO OOOO OOOO  OOOO ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>69</v>
+      <c r="D28" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>68</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G28" s="38" t="str">
+        <v>87</v>
+      </c>
+      <c r="G28" s="35" t="str">
         <f>VLOOKUP(D28,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>OO OOOO OOOO  OOOO OOOO OOOO OOOO</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="24"/>
-      <c r="C29" s="25" t="s">
+      <c r="B29" s="45"/>
+      <c r="C29" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>70</v>
+      <c r="D29" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G29" s="39" t="str">
+        <v>112</v>
+      </c>
+      <c r="G29" s="36" t="str">
         <f>VLOOKUP(D29,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
         <v>OO OOOO OOOO  OOOO ΦAAA AAΦΦ ΦCCC</v>
       </c>
@@ -1721,7 +1718,7 @@
     <mergeCell ref="B28:B29"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F29">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1735,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1747,90 +1744,90 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
+      <c r="C6" s="33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="36" t="s">
+      <c r="C11" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1854,18 +1851,18 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3">
         <f>2^D3</f>
@@ -1877,7 +1874,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4">
         <f>2^D4</f>
@@ -1889,7 +1886,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <f>2^D5</f>
@@ -1901,7 +1898,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <v>32</v>
@@ -1913,7 +1910,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7">
         <v>512</v>
@@ -1925,7 +1922,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8">
         <v>256</v>
@@ -1937,7 +1934,7 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9">
         <f>D5</f>
@@ -1950,7 +1947,7 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10">
         <v>7</v>

</xml_diff>

<commit_message>
More work on the homework
</commit_message>
<xml_diff>
--- a/Homework_1/Instructions.xlsx
+++ b/Homework_1/Instructions.xlsx
@@ -4,16 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction set" sheetId="3" r:id="rId1"/>
     <sheet name="Operands to Register map" sheetId="4" r:id="rId2"/>
     <sheet name="Specification" sheetId="5" r:id="rId3"/>
+    <sheet name="Control Signals Q2" sheetId="6" r:id="rId4"/>
+    <sheet name="Q1 Control Signals" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Control Signals Q2'!$B$2:$M$12</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Instruction set'!$A$1:$H$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Operands to Register map'!$A$1:$D$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Table2[#All]</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Specification!$A$1:$E$11</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="203">
   <si>
     <t>Instruction</t>
   </si>
@@ -361,9 +365,6 @@
     <t>DMEM[addr] &lt;= rb {direct addressing}</t>
   </si>
   <si>
-    <t>OO OOOO OOOO  OOOO OOOO OOOO OOOO</t>
-  </si>
-  <si>
     <t>11 10 00</t>
   </si>
   <si>
@@ -373,9 +374,6 @@
     <t>ΦΦ ΦΦΦΦ ΦΦΦΦ  BBBB BAAA AAΦT TTTT</t>
   </si>
   <si>
-    <t>OO OOOO OOOO  OOOO ΦAAA AAΦT TTTT</t>
-  </si>
-  <si>
     <t>ΦΦ NNNN ΦΦΦΦ  ΦΦΦΦ ΦAAA AAΦT TTTT</t>
   </si>
   <si>
@@ -388,20 +386,266 @@
     <t>II IIII IIII  IIII IIII IIΦT TTTT</t>
   </si>
   <si>
-    <t>OO OOOO OOOO  OOOO ΦAAA AAΦΦ ΦCCC</t>
-  </si>
-  <si>
     <t>AA AAAA AAAA  AAAA AAAA AAΦT TTTT</t>
   </si>
   <si>
     <t>ΦΦ ΦΦΦΦ ΦΦΦΦ  ΦΦΦΦ ΦΦΦΦ ΦΦΦΦ ΦΦΦΦ</t>
+  </si>
+  <si>
+    <t>ΦΦ ΦΦΦO OOOO  OOOO ΦAAA AAΦT TTTT</t>
+  </si>
+  <si>
+    <t>ΦΦ ΦΦΦΦ OOOO  OOOO ΦΦΦΦ ΦΦΦΦ ΦΦΦΦ</t>
+  </si>
+  <si>
+    <t>ΦΦ ΦΦΦΦ OOOO  OOOO ΦAAA AAΦΦ ΦCCC</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>ØØ000</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>00ØØ</t>
+  </si>
+  <si>
+    <t>0xØØØØ</t>
+  </si>
+  <si>
+    <t>ØØØ</t>
+  </si>
+  <si>
+    <t>S3 - ALU</t>
+  </si>
+  <si>
+    <t>11ØØ</t>
+  </si>
+  <si>
+    <t>0x011A</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>S2 - Reg R</t>
+  </si>
+  <si>
+    <t>ØØØØØ</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>Ø1ØØ</t>
+  </si>
+  <si>
+    <t>S1 - Fetch</t>
+  </si>
+  <si>
+    <t>BRNEQ R3, 0x11A</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ØØØ1</t>
+  </si>
+  <si>
+    <t>S5 - Reg W</t>
+  </si>
+  <si>
+    <t>ØØ1Ø</t>
+  </si>
+  <si>
+    <t>0xAF1F</t>
+  </si>
+  <si>
+    <t>S4 - Mem RW</t>
+  </si>
+  <si>
+    <t>LOADI R5, 0xAF1F</t>
+  </si>
+  <si>
+    <t>ØØØ0</t>
+  </si>
+  <si>
+    <t>S4 - Reg W</t>
+  </si>
+  <si>
+    <t>10101</t>
+  </si>
+  <si>
+    <t>00Ø0</t>
+  </si>
+  <si>
+    <t>ØØØØ</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>SHR R3, R1, 5</t>
+  </si>
+  <si>
+    <t>WEN</t>
+  </si>
+  <si>
+    <t>SH[5:0]</t>
+  </si>
+  <si>
+    <t>AL[2:0]</t>
+  </si>
+  <si>
+    <t>S[1:4]</t>
+  </si>
+  <si>
+    <t>OEN</t>
+  </si>
+  <si>
+    <t>IMM[15:0]</t>
+  </si>
+  <si>
+    <t>MA[15:0]</t>
+  </si>
+  <si>
+    <t>WA[2:0]</t>
+  </si>
+  <si>
+    <t>RB[2:0]</t>
+  </si>
+  <si>
+    <t>RA[2:0]</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>S[4:1]</t>
+  </si>
+  <si>
+    <t>Al[2:0]</t>
+  </si>
+  <si>
+    <t>move R2, R7</t>
+  </si>
+  <si>
+    <t>movi R3, 0x0000</t>
+  </si>
+  <si>
+    <t>move R4, R1</t>
+  </si>
+  <si>
+    <t>movi R5, 0x0001</t>
+  </si>
+  <si>
+    <t>and R6, R2, R4</t>
+  </si>
+  <si>
+    <t>xor R3, R6, R4</t>
+  </si>
+  <si>
+    <t>shr R2, R2, 1</t>
+  </si>
+  <si>
+    <t>dec R4, R4</t>
+  </si>
+  <si>
+    <t>br R4, 000, loop_end_label</t>
+  </si>
+  <si>
+    <t>br R0, 000, loop_start_label</t>
+  </si>
+  <si>
+    <t>storo R7,  R3, 2</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
+    <t>11000</t>
+  </si>
+  <si>
+    <t>01100</t>
+  </si>
+  <si>
+    <t>01110</t>
+  </si>
+  <si>
+    <t>01001</t>
+  </si>
+  <si>
+    <t>00011</t>
+  </si>
+  <si>
+    <t>10111</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>ΦΦΦ</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>0x0001</t>
+  </si>
+  <si>
+    <t>0x0005</t>
+  </si>
+  <si>
+    <t>0xΦΦΦΦ</t>
+  </si>
+  <si>
+    <t>0xFFFB</t>
+  </si>
+  <si>
+    <t>0x0002</t>
+  </si>
+  <si>
+    <t>0ΦΦ0</t>
+  </si>
+  <si>
+    <t>0ΦΦ1</t>
+  </si>
+  <si>
+    <t>ΦΦΦ1</t>
+  </si>
+  <si>
+    <t>00Φ1</t>
+  </si>
+  <si>
+    <t>ΦΦ0000</t>
+  </si>
+  <si>
+    <t>100001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,8 +672,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,8 +725,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -686,11 +975,188 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -757,11 +1223,127 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -817,16 +1399,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
@@ -850,9 +1422,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="firstColumn" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="firstColumn" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -873,10 +1445,42 @@
     <sortCondition descending="1" ref="B2:B11"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Operands" dataDxfId="1"/>
-    <tableColumn id="2" name="Fields" dataDxfId="0"/>
+    <tableColumn id="1" name="Operands" dataDxfId="12"/>
+    <tableColumn id="2" name="Fields" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:L13">
+  <autoFilter ref="B2:L13">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Command" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Opcode" dataDxfId="10"/>
+    <tableColumn id="3" name="RA[2:0]" dataDxfId="9"/>
+    <tableColumn id="4" name="RB[2:0]" dataDxfId="8"/>
+    <tableColumn id="5" name="WA[2:0]" dataDxfId="7"/>
+    <tableColumn id="6" name="IMM[15:0]" dataDxfId="6"/>
+    <tableColumn id="7" name="OEN" dataDxfId="5"/>
+    <tableColumn id="8" name="S[4:1]" dataDxfId="4"/>
+    <tableColumn id="9" name="Al[2:0]" dataDxfId="3"/>
+    <tableColumn id="10" name="SH[5:0]" dataDxfId="2"/>
+    <tableColumn id="11" name="WEN" totalsRowFunction="count" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1148,8 +1752,8 @@
   </sheetPr>
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,7 +2214,7 @@
       </c>
       <c r="G24" s="38" t="str">
         <f>VLOOKUP(D24,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
-        <v>OO OOOO OOOO  OOOO ΦAAA AAΦT TTTT</v>
+        <v>ΦΦ ΦΦΦO OOOO  OOOO ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -1667,7 +2271,7 @@
       </c>
       <c r="G27" s="36" t="str">
         <f>VLOOKUP(D27,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
-        <v>OO OOOO OOOO  OOOO ΦAAA AAΦT TTTT</v>
+        <v>ΦΦ ΦΦΦO OOOO  OOOO ΦAAA AAΦT TTTT</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -1688,7 +2292,7 @@
       </c>
       <c r="G28" s="35" t="str">
         <f>VLOOKUP(D28,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
-        <v>OO OOOO OOOO  OOOO OOOO OOOO OOOO</v>
+        <v>ΦΦ ΦΦΦΦ OOOO  OOOO ΦΦΦΦ ΦΦΦΦ ΦΦΦΦ</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1703,11 +2307,11 @@
         <v>69</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G29" s="36" t="str">
         <f>VLOOKUP(D29,'Operands to Register map'!$B$3:$C$12,2,FALSE)</f>
-        <v>OO OOOO OOOO  OOOO ΦAAA AAΦΦ ΦCCC</v>
+        <v>ΦΦ ΦΦΦΦ OOOO  OOOO ΦAAA AAΦΦ ΦCCC</v>
       </c>
     </row>
   </sheetData>
@@ -1718,7 +2322,7 @@
     <mergeCell ref="B28:B29"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F29">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1733,7 +2337,7 @@
   <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,7 +2359,7 @@
         <v>33</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1763,7 +2367,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -1771,7 +2375,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1779,7 +2383,7 @@
         <v>34</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1787,7 +2391,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1795,7 +2399,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1803,7 +2407,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -1811,7 +2415,7 @@
         <v>108</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
@@ -1819,7 +2423,7 @@
         <v>39</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -1827,7 +2431,7 @@
         <v>107</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1844,10 +2448,14 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
@@ -1947,7 +2555,7 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -1961,4 +2569,897 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:M12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="I2" s="71" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="L2" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="M2" s="70" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="69" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="67">
+        <v>0</v>
+      </c>
+      <c r="J3" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" s="67">
+        <v>111</v>
+      </c>
+      <c r="L3" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="M3" s="66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="53"/>
+      <c r="C4" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>151</v>
+      </c>
+      <c r="K4" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="L4" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="M4" s="50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="53"/>
+      <c r="C5" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="K5" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="L5" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="M5" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="53"/>
+      <c r="C6" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="K6" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="M6" s="50" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="63" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="K7" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="L7" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="M7" s="62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="61"/>
+      <c r="C8" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="H8" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="K8" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="L8" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="M8" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="60"/>
+      <c r="C9" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="K9" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="L9" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="M9" s="57" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="J10" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="K10" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="L10" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="M10" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="53"/>
+      <c r="C11" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="I11" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="J11" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="L11" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="M11" s="50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="49"/>
+      <c r="C12" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="K12" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="L12" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="M12" s="46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="73">
+        <v>10001</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="G3" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="H3" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="J3" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K3" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L3" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="73" t="s">
+        <v>191</v>
+      </c>
+      <c r="H4" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="73" t="s">
+        <v>198</v>
+      </c>
+      <c r="J4" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K4" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="H5" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K5" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L5" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="73" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="73" t="s">
+        <v>198</v>
+      </c>
+      <c r="J6" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L6" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>189</v>
+      </c>
+      <c r="E7" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="G7" s="73" t="s">
+        <v>193</v>
+      </c>
+      <c r="H7" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="73" t="s">
+        <v>199</v>
+      </c>
+      <c r="J7" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L7" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="73" t="s">
+        <v>189</v>
+      </c>
+      <c r="F8" s="73" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="H8" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="J8" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="K8" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L8" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" s="73" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="H9" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="J9" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="K9" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L9" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="G10" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="H10" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="J10" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K10" s="73" t="s">
+        <v>202</v>
+      </c>
+      <c r="L10" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="73" t="s">
+        <v>189</v>
+      </c>
+      <c r="E11" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="F11" s="73" t="s">
+        <v>189</v>
+      </c>
+      <c r="G11" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="H11" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="J11" s="73" t="s">
+        <v>189</v>
+      </c>
+      <c r="K11" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L11" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12" s="73" t="s">
+        <v>195</v>
+      </c>
+      <c r="H12" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" s="73" t="s">
+        <v>199</v>
+      </c>
+      <c r="J12" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K12" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L12" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="G13" s="73" t="s">
+        <v>196</v>
+      </c>
+      <c r="H13" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13" s="73" t="s">
+        <v>200</v>
+      </c>
+      <c r="J13" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K13" s="73" t="s">
+        <v>201</v>
+      </c>
+      <c r="L13" s="73" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>